<commit_message>
adding correct data and fixing spacing
Signed-off-by: YelloElefant <alextrotternz@gmail.com>
</commit_message>
<xml_diff>
--- a/Assets/u15tournamentwebsitestuff/2023 Pools .xlsx
+++ b/Assets/u15tournamentwebsitestuff/2023 Pools .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewh/Desktop/bits n bobs /U15 Torneo 2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a04a139e370f3223/Coding/13IA/Assets/u15tournamentwebsitestuff/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7687326-D7BA-4245-B1C1-E3C4F3EF0494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{F7687326-D7BA-4245-B1C1-E3C4F3EF0494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C4419D0-6E8F-452F-81BF-3DB058F5E38F}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="920" windowWidth="27640" windowHeight="15760" xr2:uid="{8FB1341E-E18F-D840-BB43-BE3D5F47C884}"/>
+    <workbookView xWindow="-28920" yWindow="1050" windowWidth="29040" windowHeight="15840" xr2:uid="{8FB1341E-E18F-D840-BB43-BE3D5F47C884}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="1" r:id="rId1"/>
@@ -952,21 +952,21 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G3" sqref="G3:G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="29" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="29.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="75.1640625" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="75.125" customWidth="1"/>
+    <col min="4" max="4" width="20.375" customWidth="1"/>
+    <col min="5" max="5" width="17.375" customWidth="1"/>
+    <col min="6" max="6" width="15.375" customWidth="1"/>
+    <col min="7" max="7" width="23.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6">
         <v>2022</v>
       </c>
@@ -977,7 +977,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -998,7 +998,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>23</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>24</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>25</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>26</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>27</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>28</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>29</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>30</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>31</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>32</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>33</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>34</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>35</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>36</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>37</v>
       </c>
@@ -1224,6 +1224,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>